<commit_message>
Fixing bugs in SLO estimator
</commit_message>
<xml_diff>
--- a/slo-estimation-tool/Composite_SLO_Estimation_Tool.xlsx
+++ b/slo-estimation-tool/Composite_SLO_Estimation_Tool.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C27E464-40D8-4169-83EA-5F222A3B37CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F662193-836F-4ABA-9576-81A76BF4D1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{FEC4E9EF-0B4B-44BF-B15A-D353C80B4A94}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{FEC4E9EF-0B4B-44BF-B15A-D353C80B4A94}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Traffic Manager</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>READ BEFORE USING THIS TOOL</t>
+  </si>
+  <si>
+    <t>Azure SLA's can be read as SLOs</t>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-au/support/legal/sla/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tEylFyxbDLE</t>
+  </si>
+  <si>
+    <t>SLIs, SLOs, SLAs, oh my!</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -404,19 +416,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -735,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DFAEB0-461E-4E42-878E-6B9140A7055E}">
   <dimension ref="B1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -745,17 +754,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="48" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>20</v>
       </c>
     </row>
@@ -769,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFCC544-15F4-4DCC-826B-B523B3F5E623}">
   <dimension ref="B2:V35"/>
   <sheetViews>
-    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -954,6 +963,7 @@
       <c r="P8" s="12"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="30">
+        <f>H8</f>
         <v>0.99950000000000006</v>
       </c>
       <c r="S8" s="14"/>
@@ -994,11 +1004,11 @@
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="49" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="49" t="s">
         <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1010,11 +1020,11 @@
       <c r="L10" s="13"/>
       <c r="M10" s="11"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="47" t="s">
+      <c r="O10" s="49" t="s">
         <v>3</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="47" t="s">
+      <c r="Q10" s="49" t="s">
         <v>4</v>
       </c>
       <c r="R10" s="29" t="str">
@@ -1028,9 +1038,9 @@
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="47"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="47"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="5">
         <v>0.99950000000000006</v>
       </c>
@@ -1040,15 +1050,18 @@
       <c r="L11" s="13"/>
       <c r="M11" s="11"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="47"/>
+      <c r="O11" s="49"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="47"/>
+      <c r="Q11" s="49"/>
       <c r="R11" s="30">
         <f>H11</f>
         <v>0.99950000000000006</v>
       </c>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
+      <c r="V11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B12" s="11"/>
@@ -1074,6 +1087,9 @@
       </c>
       <c r="S12" s="14"/>
       <c r="T12" s="14"/>
+      <c r="V12" s="42" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
@@ -1081,13 +1097,13 @@
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="49" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="49" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="3" t="s">
@@ -1102,14 +1118,14 @@
         <f>D13</f>
         <v>App Service</v>
       </c>
-      <c r="O13" s="47" t="s">
+      <c r="O13" s="49" t="s">
         <v>3</v>
       </c>
       <c r="P13" s="3" t="str">
         <f>F13</f>
         <v>Key Vault</v>
       </c>
-      <c r="Q13" s="47" t="s">
+      <c r="Q13" s="49" t="s">
         <v>4</v>
       </c>
       <c r="R13" s="3" t="str">
@@ -1118,6 +1134,9 @@
       </c>
       <c r="S13" s="14"/>
       <c r="T13" s="14"/>
+      <c r="V13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
@@ -1125,14 +1144,14 @@
       <c r="D14" s="5">
         <v>0.99950000000000006</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="4">
         <v>0.999</v>
       </c>
-      <c r="G14" s="47"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="5">
-        <f>D14</f>
-        <v>0.99950000000000006</v>
+        <f>D14*F14</f>
+        <v>0.99850050000000001</v>
       </c>
       <c r="I14" s="23"/>
       <c r="J14" s="13"/>
@@ -1143,18 +1162,21 @@
         <f>D14</f>
         <v>0.99950000000000006</v>
       </c>
-      <c r="O14" s="47"/>
+      <c r="O14" s="49"/>
       <c r="P14" s="4">
         <f>F14</f>
         <v>0.999</v>
       </c>
-      <c r="Q14" s="47"/>
+      <c r="Q14" s="49"/>
       <c r="R14" s="5">
-        <f>H14</f>
-        <v>0.99950000000000006</v>
+        <f>N14*P14</f>
+        <v>0.99850050000000001</v>
       </c>
       <c r="S14" s="14"/>
       <c r="T14" s="14"/>
+      <c r="V14" s="42" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
@@ -1519,7 +1541,7 @@
       <c r="G29" s="13"/>
       <c r="H29" s="44">
         <f>H8*H11*H14*H17*H20*H23*H26</f>
-        <v>0.99739277447295271</v>
+        <v>0.99639538169847985</v>
       </c>
       <c r="I29" s="12"/>
       <c r="J29" s="13"/>
@@ -1530,9 +1552,9 @@
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="13"/>
-      <c r="R29" s="46">
-        <f>H29</f>
-        <v>0.99739277447295271</v>
+      <c r="R29" s="44">
+        <f>R8*R11*R14*R17*R20*R23*R26</f>
+        <v>0.99639538169847985</v>
       </c>
       <c r="S29" s="13"/>
       <c r="T29" s="14"/>
@@ -1593,7 +1615,7 @@
       <c r="J32" s="18"/>
       <c r="K32" s="41">
         <f>(1-((1-H29)*(1-R29)))*K4</f>
-        <v>0.99989320305481355</v>
+        <v>0.99988700802622765</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -1628,8 +1650,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B35" r:id="rId1" xr:uid="{CA025AB8-DC93-41FF-A6C4-C4B1BF3FE19D}"/>
+    <hyperlink ref="V12" r:id="rId2" xr:uid="{F26A7EF2-CAA8-4123-A7EA-C1C7C9496A0C}"/>
+    <hyperlink ref="V14" r:id="rId3" xr:uid="{C6D7FAA9-1C13-427A-912F-EE5BED5816B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>